<commit_message>
CreateShaderResourceView 오류 해결 필요
</commit_message>
<xml_diff>
--- a/Doc/데이터 정리.xlsx
+++ b/Doc/데이터 정리.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1574e86df6b37cf/Kyun/01_PROJECT/26_DirectX12/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{C86A9A51-E514-413A-AC42-586636D63F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{321B46C1-4485-4709-8114-3BE44DD5A707}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{C86A9A51-E514-413A-AC42-586636D63F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{293F44A3-BDAF-4A50-ADE6-FF53D3F1C707}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="0" windowWidth="46056" windowHeight="25320" activeTab="2" xr2:uid="{42312EC7-06E0-49F0-84AA-5D15BB2763A2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="175">
   <si>
     <t>InstanceData</t>
   </si>
@@ -559,6 +559,18 @@
   </si>
   <si>
     <t>lock 간 중간 단계 오류 해결</t>
+  </si>
+  <si>
+    <t>TX USIT SBC EQ 동작 검증</t>
+  </si>
+  <si>
+    <t>TX USIT SBC Error 동작 검증</t>
+  </si>
+  <si>
+    <t>TX USIT RD2 동작 검증</t>
+  </si>
+  <si>
+    <t>CreateShaderResourceView 오류 해결</t>
   </si>
 </sst>
 </file>
@@ -2846,7 +2858,7 @@
   <dimension ref="A1:AS45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="AE1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AI33" sqref="AI33"/>
+      <selection activeCell="AG15" sqref="AG15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.8" x14ac:dyDescent="0.3"/>
@@ -3275,7 +3287,9 @@
       <c r="AB8" s="19"/>
       <c r="AC8" s="46"/>
       <c r="AD8" s="19"/>
-      <c r="AF8" s="46"/>
+      <c r="AF8" s="46" t="s">
+        <v>110</v>
+      </c>
       <c r="AG8" s="19" t="s">
         <v>155</v>
       </c>
@@ -3545,7 +3559,9 @@
       <c r="AD13" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="AF13" s="46"/>
+      <c r="AF13" s="46" t="s">
+        <v>110</v>
+      </c>
       <c r="AG13" s="19" t="s">
         <v>170</v>
       </c>
@@ -3654,7 +3670,9 @@
         <v>168</v>
       </c>
       <c r="AF15" s="46"/>
-      <c r="AG15" s="19"/>
+      <c r="AG15" s="19" t="s">
+        <v>174</v>
+      </c>
       <c r="AH15" s="46"/>
       <c r="AI15" s="19"/>
       <c r="AJ15" s="46"/>
@@ -4370,7 +4388,9 @@
       <c r="AF27" s="46">
         <v>9</v>
       </c>
-      <c r="AG27" s="19"/>
+      <c r="AG27" s="19" t="s">
+        <v>171</v>
+      </c>
       <c r="AH27" s="46">
         <v>9</v>
       </c>
@@ -4472,7 +4492,9 @@
       <c r="AF28" s="46">
         <v>10</v>
       </c>
-      <c r="AG28" s="19"/>
+      <c r="AG28" s="19" t="s">
+        <v>171</v>
+      </c>
       <c r="AH28" s="46">
         <v>10</v>
       </c>
@@ -4576,7 +4598,9 @@
       <c r="AF29" s="46">
         <v>11</v>
       </c>
-      <c r="AG29" s="19"/>
+      <c r="AG29" s="19" t="s">
+        <v>171</v>
+      </c>
       <c r="AH29" s="46">
         <v>11</v>
       </c>
@@ -4680,7 +4704,9 @@
       <c r="AF30" s="46">
         <v>12</v>
       </c>
-      <c r="AG30" s="19"/>
+      <c r="AG30" s="19" t="s">
+        <v>171</v>
+      </c>
       <c r="AH30" s="46">
         <v>12</v>
       </c>
@@ -4784,7 +4810,9 @@
       <c r="AF31" s="46">
         <v>1</v>
       </c>
-      <c r="AG31" s="19"/>
+      <c r="AG31" s="19" t="s">
+        <v>172</v>
+      </c>
       <c r="AH31" s="46">
         <v>1</v>
       </c>
@@ -4888,7 +4916,9 @@
       <c r="AF32" s="46">
         <v>2</v>
       </c>
-      <c r="AG32" s="19"/>
+      <c r="AG32" s="19" t="s">
+        <v>172</v>
+      </c>
       <c r="AH32" s="46">
         <v>2</v>
       </c>
@@ -4992,7 +5022,9 @@
       <c r="AF33" s="46">
         <v>3</v>
       </c>
-      <c r="AG33" s="19"/>
+      <c r="AG33" s="19" t="s">
+        <v>172</v>
+      </c>
       <c r="AH33" s="46">
         <v>3</v>
       </c>
@@ -5094,7 +5126,9 @@
       <c r="AF34" s="46">
         <v>4</v>
       </c>
-      <c r="AG34" s="19"/>
+      <c r="AG34" s="19" t="s">
+        <v>172</v>
+      </c>
       <c r="AH34" s="46">
         <v>4</v>
       </c>
@@ -5194,7 +5228,9 @@
       <c r="AF35" s="46">
         <v>5</v>
       </c>
-      <c r="AG35" s="19"/>
+      <c r="AG35" s="19" t="s">
+        <v>172</v>
+      </c>
       <c r="AH35" s="46">
         <v>5</v>
       </c>
@@ -5296,7 +5332,9 @@
       <c r="AF36" s="46">
         <v>6</v>
       </c>
-      <c r="AG36" s="19"/>
+      <c r="AG36" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="AH36" s="46">
         <v>6</v>
       </c>
@@ -5398,7 +5436,9 @@
       <c r="AF37" s="46">
         <v>7</v>
       </c>
-      <c r="AG37" s="19"/>
+      <c r="AG37" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="AH37" s="46">
         <v>7</v>
       </c>
@@ -5500,7 +5540,9 @@
       <c r="AF38" s="46">
         <v>8</v>
       </c>
-      <c r="AG38" s="19"/>
+      <c r="AG38" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="AH38" s="46">
         <v>8</v>
       </c>
@@ -5594,7 +5636,9 @@
       <c r="AF39" s="46">
         <v>9</v>
       </c>
-      <c r="AG39" s="19"/>
+      <c r="AG39" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="AH39" s="46">
         <v>9</v>
       </c>
@@ -5694,7 +5738,9 @@
       <c r="AF40" s="46">
         <v>10</v>
       </c>
-      <c r="AG40" s="19"/>
+      <c r="AG40" s="19" t="s">
+        <v>173</v>
+      </c>
       <c r="AH40" s="46">
         <v>10</v>
       </c>
@@ -5790,7 +5836,9 @@
       <c r="AF41" s="46">
         <v>11</v>
       </c>
-      <c r="AG41" s="19"/>
+      <c r="AG41" s="19" t="s">
+        <v>170</v>
+      </c>
       <c r="AH41" s="46">
         <v>11</v>
       </c>
@@ -5890,7 +5938,9 @@
       <c r="AF42" s="46">
         <v>12</v>
       </c>
-      <c r="AG42" s="19"/>
+      <c r="AG42" s="19" t="s">
+        <v>174</v>
+      </c>
       <c r="AH42" s="46">
         <v>12</v>
       </c>
@@ -5984,7 +6034,9 @@
       <c r="AF43" s="46">
         <v>1</v>
       </c>
-      <c r="AG43" s="19"/>
+      <c r="AG43" s="19" t="s">
+        <v>174</v>
+      </c>
       <c r="AH43" s="46">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Markdown 문서 작성 with Copilot
</commit_message>
<xml_diff>
--- a/Doc/데이터 정리.xlsx
+++ b/Doc/데이터 정리.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1574e86df6b37cf/Kyun/01_PROJECT/26_DirectX12/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="13_ncr:1_{C86A9A51-E514-413A-AC42-586636D63F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4282E5E1-803E-44CD-8C8A-2B0A1D5D8F2B}"/>
+  <xr:revisionPtr revIDLastSave="190" documentId="13_ncr:1_{C86A9A51-E514-413A-AC42-586636D63F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C94C5E56-D442-4127-93AC-52A5DDCDCF43}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-108" windowWidth="46296" windowHeight="25536" activeTab="2" xr2:uid="{42312EC7-06E0-49F0-84AA-5D15BB2763A2}"/>
+    <workbookView xWindow="46104" yWindow="0" windowWidth="46056" windowHeight="25320" activeTab="2" xr2:uid="{42312EC7-06E0-49F0-84AA-5D15BB2763A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Struct" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="200">
   <si>
     <t>InstanceData</t>
   </si>
@@ -644,6 +644,9 @@
   </si>
   <si>
     <t>JSON 연동 파일 저장 구현</t>
+  </si>
+  <si>
+    <t>저장 로직 개선</t>
   </si>
 </sst>
 </file>
@@ -2934,7 +2937,7 @@
   <dimension ref="A1:BW46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="AT1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AY18" sqref="AY18"/>
+      <selection activeCell="BA13" sqref="BA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="10.8" x14ac:dyDescent="0.3"/>
@@ -3979,8 +3982,12 @@
       <c r="AZ12" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="BA12" s="46"/>
-      <c r="BB12" s="19"/>
+      <c r="BA12" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="BB12" s="19" t="s">
+        <v>199</v>
+      </c>
       <c r="BC12" s="46"/>
       <c r="BD12" s="19"/>
       <c r="BE12" s="46"/>
@@ -4092,7 +4099,9 @@
         <v>183</v>
       </c>
       <c r="BA13" s="46"/>
-      <c r="BB13" s="19"/>
+      <c r="BB13" s="19" t="s">
+        <v>183</v>
+      </c>
       <c r="BC13" s="46"/>
       <c r="BD13" s="19"/>
       <c r="BE13" s="46"/>
@@ -4188,7 +4197,9 @@
         <v>189</v>
       </c>
       <c r="BA14" s="46"/>
-      <c r="BB14" s="19"/>
+      <c r="BB14" s="19" t="s">
+        <v>190</v>
+      </c>
       <c r="BC14" s="46"/>
       <c r="BD14" s="19"/>
       <c r="BE14" s="46"/>
@@ -5554,7 +5565,9 @@
       <c r="BA28" s="46">
         <v>9</v>
       </c>
-      <c r="BB28" s="19"/>
+      <c r="BB28" s="19" t="s">
+        <v>176</v>
+      </c>
       <c r="BC28" s="46">
         <v>9</v>
       </c>
@@ -5730,7 +5743,9 @@
       <c r="BA29" s="46">
         <v>10</v>
       </c>
-      <c r="BB29" s="19"/>
+      <c r="BB29" s="19" t="s">
+        <v>176</v>
+      </c>
       <c r="BC29" s="46">
         <v>10</v>
       </c>
@@ -5908,7 +5923,9 @@
       <c r="BA30" s="46">
         <v>11</v>
       </c>
-      <c r="BB30" s="19"/>
+      <c r="BB30" s="19" t="s">
+        <v>176</v>
+      </c>
       <c r="BC30" s="46">
         <v>11</v>
       </c>
@@ -6088,7 +6105,9 @@
       <c r="BA31" s="46">
         <v>12</v>
       </c>
-      <c r="BB31" s="19"/>
+      <c r="BB31" s="19" t="s">
+        <v>176</v>
+      </c>
       <c r="BC31" s="46">
         <v>12</v>
       </c>
@@ -6268,7 +6287,9 @@
       <c r="BA32" s="46">
         <v>1</v>
       </c>
-      <c r="BB32" s="19"/>
+      <c r="BB32" s="19" t="s">
+        <v>176</v>
+      </c>
       <c r="BC32" s="46">
         <v>1</v>
       </c>
@@ -6448,7 +6469,9 @@
       <c r="BA33" s="46">
         <v>2</v>
       </c>
-      <c r="BB33" s="19"/>
+      <c r="BB33" s="19" t="s">
+        <v>176</v>
+      </c>
       <c r="BC33" s="46">
         <v>2</v>
       </c>
@@ -6628,7 +6651,9 @@
       <c r="BA34" s="46">
         <v>3</v>
       </c>
-      <c r="BB34" s="19"/>
+      <c r="BB34" s="19" t="s">
+        <v>176</v>
+      </c>
       <c r="BC34" s="46">
         <v>3</v>
       </c>
@@ -6806,7 +6831,9 @@
       <c r="BA35" s="46">
         <v>4</v>
       </c>
-      <c r="BB35" s="19"/>
+      <c r="BB35" s="19" t="s">
+        <v>176</v>
+      </c>
       <c r="BC35" s="46">
         <v>4</v>
       </c>
@@ -6982,7 +7009,9 @@
       <c r="BA36" s="46">
         <v>5</v>
       </c>
-      <c r="BB36" s="19"/>
+      <c r="BB36" s="19" t="s">
+        <v>176</v>
+      </c>
       <c r="BC36" s="46">
         <v>5</v>
       </c>
@@ -7160,7 +7189,9 @@
       <c r="BA37" s="46">
         <v>6</v>
       </c>
-      <c r="BB37" s="19"/>
+      <c r="BB37" s="19" t="s">
+        <v>176</v>
+      </c>
       <c r="BC37" s="46">
         <v>6</v>
       </c>
@@ -7336,7 +7367,9 @@
       <c r="BA38" s="46">
         <v>7</v>
       </c>
-      <c r="BB38" s="19"/>
+      <c r="BB38" s="19" t="s">
+        <v>152</v>
+      </c>
       <c r="BC38" s="46">
         <v>7</v>
       </c>
@@ -7514,7 +7547,9 @@
       <c r="BA39" s="46">
         <v>8</v>
       </c>
-      <c r="BB39" s="19"/>
+      <c r="BB39" s="19" t="s">
+        <v>152</v>
+      </c>
       <c r="BC39" s="46">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
System별 Repectoring 진행 및 System 정리 자료 작성 중
</commit_message>
<xml_diff>
--- a/Doc/데이터 정리.xlsx
+++ b/Doc/데이터 정리.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1574e86df6b37cf/Kyun/01_PROJECT/26_DirectX12/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="13_ncr:1_{C86A9A51-E514-413A-AC42-586636D63F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C94C5E56-D442-4127-93AC-52A5DDCDCF43}"/>
+  <xr:revisionPtr revIDLastSave="385" documentId="13_ncr:1_{C86A9A51-E514-413A-AC42-586636D63F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20570902-62C9-49C3-BD25-4CD20B0A598D}"/>
   <bookViews>
-    <workbookView xWindow="46104" yWindow="0" windowWidth="46056" windowHeight="25320" activeTab="2" xr2:uid="{42312EC7-06E0-49F0-84AA-5D15BB2763A2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14532" windowHeight="25320" activeTab="2" xr2:uid="{42312EC7-06E0-49F0-84AA-5D15BB2763A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Struct" sheetId="1" r:id="rId1"/>
     <sheet name="Function" sheetId="2" r:id="rId2"/>
-    <sheet name="일정" sheetId="4" r:id="rId3"/>
+    <sheet name="System" sheetId="6" r:id="rId3"/>
+    <sheet name="일정" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1011" uniqueCount="257">
   <si>
     <t>InstanceData</t>
   </si>
@@ -647,6 +648,179 @@
   </si>
   <si>
     <t>저장 로직 개선</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>FMODAudioSystem</t>
+  </si>
+  <si>
+    <t>FMODAudioComponent</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>bool loop;</t>
+  </si>
+  <si>
+    <t>float volume;</t>
+  </si>
+  <si>
+    <t>AudioHandle (size_t)</t>
+  </si>
+  <si>
+    <t>PhysicsSystem</t>
+  </si>
+  <si>
+    <t>TransformComponent</t>
+  </si>
+  <si>
+    <t>float4</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Rotation</t>
+  </si>
+  <si>
+    <t>RotationQuat</t>
+  </si>
+  <si>
+    <t>RigidBodyComponent</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>DiffPosition</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>AngularVelocity</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Torque</t>
+  </si>
+  <si>
+    <t>Acceleration</t>
+  </si>
+  <si>
+    <t>AngularAcceleration</t>
+  </si>
+  <si>
+    <t>UseGravity</t>
+  </si>
+  <si>
+    <t>IsKinematic</t>
+  </si>
+  <si>
+    <t>GravityComponent</t>
+  </si>
+  <si>
+    <t>Audio 출력 관리</t>
+  </si>
+  <si>
+    <t>물체 이동 관리</t>
+  </si>
+  <si>
+    <t>LightSystem</t>
+  </si>
+  <si>
+    <t>DirectX::SimpleMath::Vector3</t>
+  </si>
+  <si>
+    <t>LightComponent</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>FalloffStart</t>
+  </si>
+  <si>
+    <t>FalloffEnd</t>
+  </si>
+  <si>
+    <t>SpotPower</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>eLightType</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>haloRadius</t>
+  </si>
+  <si>
+    <t>haloStrength</t>
+  </si>
+  <si>
+    <t>DX12_BoundingSystem</t>
+  </si>
+  <si>
+    <t>DX12_BoundingComponent</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>Sphere</t>
+  </si>
+  <si>
+    <t>BoundingVolumeUpdateSystem</t>
+  </si>
+  <si>
+    <t>Base Data</t>
+  </si>
+  <si>
+    <t>Instance 별 데이터</t>
+  </si>
+  <si>
+    <t>PlayerControlSystem</t>
+  </si>
+  <si>
+    <t>moveSpeed</t>
+  </si>
+  <si>
+    <t>PlayerControlComponent</t>
+  </si>
+  <si>
+    <t>RenderDataSyncSystem</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Final Update</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>RigidBody 정보 업데이트</t>
+  </si>
+  <si>
+    <t>RigidBody 정보에 따른 Transform 정보 업데이트
++
+업데이트 발생 시 Dirty Flag 제어</t>
   </si>
 </sst>
 </file>
@@ -657,7 +831,7 @@
     <numFmt numFmtId="164" formatCode="ddd\ \ d"/>
     <numFmt numFmtId="165" formatCode="m/d\ \[ddd\]"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -684,6 +858,24 @@
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Noto Sans KR Medium"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Noto Sans KR Medium"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Noto Sans KR Black"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -718,7 +910,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1001,11 +1193,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1123,6 +1352,75 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1460,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2829DBA9-5371-49D6-92D0-267134EE5124}">
   <dimension ref="B1:R82"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2319,7 +2617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA21CF0-8236-4A40-BA73-8D682A484C77}">
   <dimension ref="B1:D66"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2933,10 +3231,1516 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D5F00D-32C1-46CE-A27E-DD70C762CAB5}">
+  <dimension ref="B1:S114"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36:F56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="0.88671875" style="49" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" style="48" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" style="48" customWidth="1"/>
+    <col min="6" max="7" width="16" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="48" bestFit="1" customWidth="1"/>
+    <col min="9" max="19" width="9.21875" style="48" customWidth="1"/>
+    <col min="20" max="16384" width="8.88671875" style="49"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" s="48" customFormat="1" ht="4.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+    </row>
+    <row r="2" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="52" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="52" t="s">
+        <v>204</v>
+      </c>
+      <c r="F2" s="52" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" s="52" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="53" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" s="55" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>226</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="57"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>206</v>
+      </c>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+    </row>
+    <row r="5" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="61"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>205</v>
+      </c>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+    </row>
+    <row r="6" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="53" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>209</v>
+      </c>
+      <c r="D6" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="F6" s="56" t="s">
+        <v>255</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="57"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+    </row>
+    <row r="8" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="57"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="F8" s="60"/>
+      <c r="G8" s="60"/>
+    </row>
+    <row r="9" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="57"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E9" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+    </row>
+    <row r="10" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="57"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+    </row>
+    <row r="11" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="57"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+    </row>
+    <row r="12" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="57"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+    </row>
+    <row r="13" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="57"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E13" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+    </row>
+    <row r="14" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="57"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+    </row>
+    <row r="15" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="57"/>
+      <c r="C15" s="66" t="s">
+        <v>214</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+    </row>
+    <row r="16" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="57"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>216</v>
+      </c>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+    </row>
+    <row r="17" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="57"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="59" t="s">
+        <v>217</v>
+      </c>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+    </row>
+    <row r="18" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+    </row>
+    <row r="19" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="57"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+    </row>
+    <row r="20" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="57"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+    </row>
+    <row r="21" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="57"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60"/>
+    </row>
+    <row r="22" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="57"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+    </row>
+    <row r="23" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="57"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+    </row>
+    <row r="24" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="57"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+    </row>
+    <row r="25" spans="2:7" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="61"/>
+      <c r="C25" s="67" t="s">
+        <v>225</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="63" t="s">
+        <v>219</v>
+      </c>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+    </row>
+    <row r="26" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="53" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" s="54" t="s">
+        <v>230</v>
+      </c>
+      <c r="D26" s="55" t="s">
+        <v>229</v>
+      </c>
+      <c r="E26" s="55" t="s">
+        <v>231</v>
+      </c>
+      <c r="F26" s="56"/>
+      <c r="G26" s="56"/>
+    </row>
+    <row r="27" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="57"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="59" t="s">
+        <v>232</v>
+      </c>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+    </row>
+    <row r="28" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="57"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="E28" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+    </row>
+    <row r="29" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="57"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="59" t="s">
+        <v>233</v>
+      </c>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+    </row>
+    <row r="30" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="57"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="E30" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+    </row>
+    <row r="31" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="57"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+    </row>
+    <row r="32" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="57"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="E32" s="59" t="s">
+        <v>237</v>
+      </c>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+    </row>
+    <row r="33" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="57"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="59" t="s">
+        <v>238</v>
+      </c>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+    </row>
+    <row r="34" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="57"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="59" t="s">
+        <v>239</v>
+      </c>
+      <c r="F34" s="60"/>
+      <c r="G34" s="60"/>
+    </row>
+    <row r="35" spans="2:7" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="61"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="59" t="s">
+        <v>240</v>
+      </c>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+    </row>
+    <row r="36" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="53" t="s">
+        <v>241</v>
+      </c>
+      <c r="C36" s="54" t="s">
+        <v>209</v>
+      </c>
+      <c r="D36" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+    </row>
+    <row r="37" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="57"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="F37" s="60"/>
+      <c r="G37" s="60"/>
+    </row>
+    <row r="38" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="57"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+    </row>
+    <row r="39" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="57"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E39" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="F39" s="60"/>
+      <c r="G39" s="60"/>
+    </row>
+    <row r="40" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="57"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" s="60"/>
+      <c r="G40" s="60"/>
+    </row>
+    <row r="41" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="57"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
+    </row>
+    <row r="42" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="57"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="F42" s="60"/>
+      <c r="G42" s="60"/>
+    </row>
+    <row r="43" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="57"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E43" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
+    </row>
+    <row r="44" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="57"/>
+      <c r="C44" s="65"/>
+      <c r="D44" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F44" s="60"/>
+      <c r="G44" s="60"/>
+    </row>
+    <row r="45" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="57"/>
+      <c r="C45" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="F45" s="60"/>
+      <c r="G45" s="60"/>
+    </row>
+    <row r="46" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="57"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" s="60"/>
+      <c r="G46" s="60"/>
+    </row>
+    <row r="47" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="57"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="F47" s="60"/>
+      <c r="G47" s="60"/>
+    </row>
+    <row r="48" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="57"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="60"/>
+      <c r="G48" s="60"/>
+    </row>
+    <row r="49" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="57"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="E49" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
+    </row>
+    <row r="50" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="57"/>
+      <c r="C50" s="58"/>
+      <c r="D50" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="60"/>
+      <c r="G50" s="60"/>
+    </row>
+    <row r="51" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="57"/>
+      <c r="C51" s="65"/>
+      <c r="D51" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="60"/>
+      <c r="G51" s="60"/>
+    </row>
+    <row r="52" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="57"/>
+      <c r="C52" s="66" t="s">
+        <v>242</v>
+      </c>
+      <c r="D52" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="E52" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="F52" s="60"/>
+      <c r="G52" s="60"/>
+    </row>
+    <row r="53" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="57"/>
+      <c r="C53" s="58"/>
+      <c r="D53" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" s="59" t="s">
+        <v>244</v>
+      </c>
+      <c r="F53" s="60"/>
+      <c r="G53" s="60"/>
+    </row>
+    <row r="54" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="57"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54" s="60"/>
+      <c r="G54" s="60"/>
+    </row>
+    <row r="55" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="57"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="F55" s="60"/>
+      <c r="G55" s="60"/>
+    </row>
+    <row r="56" spans="2:7" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="61"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56" s="63" t="s">
+        <v>127</v>
+      </c>
+      <c r="F56" s="64"/>
+      <c r="G56" s="64"/>
+    </row>
+    <row r="57" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="53" t="s">
+        <v>245</v>
+      </c>
+      <c r="C57" s="54" t="s">
+        <v>209</v>
+      </c>
+      <c r="D57" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="F57" s="68"/>
+      <c r="G57" s="68"/>
+    </row>
+    <row r="58" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="57"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="F58" s="69"/>
+      <c r="G58" s="69"/>
+    </row>
+    <row r="59" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="57"/>
+      <c r="C59" s="58"/>
+      <c r="D59" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="F59" s="69"/>
+      <c r="G59" s="69"/>
+    </row>
+    <row r="60" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="57"/>
+      <c r="C60" s="58"/>
+      <c r="D60" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E60" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="F60" s="69"/>
+      <c r="G60" s="69"/>
+    </row>
+    <row r="61" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="57"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E61" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F61" s="69"/>
+      <c r="G61" s="69"/>
+    </row>
+    <row r="62" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="57"/>
+      <c r="C62" s="58"/>
+      <c r="D62" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E62" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="F62" s="69"/>
+      <c r="G62" s="69"/>
+    </row>
+    <row r="63" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="57"/>
+      <c r="C63" s="58"/>
+      <c r="D63" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E63" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="F63" s="69"/>
+      <c r="G63" s="69"/>
+    </row>
+    <row r="64" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="57"/>
+      <c r="C64" s="58"/>
+      <c r="D64" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E64" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="F64" s="69"/>
+      <c r="G64" s="69"/>
+    </row>
+    <row r="65" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="57"/>
+      <c r="C65" s="65"/>
+      <c r="D65" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E65" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F65" s="69"/>
+      <c r="G65" s="69"/>
+    </row>
+    <row r="66" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="57"/>
+      <c r="C66" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="D66" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E66" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="F66" s="69"/>
+      <c r="G66" s="69"/>
+    </row>
+    <row r="67" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="57"/>
+      <c r="C67" s="58"/>
+      <c r="D67" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E67" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="F67" s="69"/>
+      <c r="G67" s="69"/>
+    </row>
+    <row r="68" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="57"/>
+      <c r="C68" s="58"/>
+      <c r="D68" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E68" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="F68" s="69"/>
+      <c r="G68" s="69"/>
+    </row>
+    <row r="69" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="57"/>
+      <c r="C69" s="58"/>
+      <c r="D69" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="F69" s="69"/>
+      <c r="G69" s="69"/>
+    </row>
+    <row r="70" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="57"/>
+      <c r="C70" s="58"/>
+      <c r="D70" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="E70" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="F70" s="69"/>
+      <c r="G70" s="69"/>
+    </row>
+    <row r="71" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="57"/>
+      <c r="C71" s="58"/>
+      <c r="D71" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="E71" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="F71" s="69" t="s">
+        <v>246</v>
+      </c>
+      <c r="G71" s="69" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="57"/>
+      <c r="C72" s="65"/>
+      <c r="D72" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F72" s="69" t="s">
+        <v>246</v>
+      </c>
+      <c r="G72" s="69" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="57"/>
+      <c r="C73" s="66" t="s">
+        <v>242</v>
+      </c>
+      <c r="D73" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="E73" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="F73" s="69" t="s">
+        <v>247</v>
+      </c>
+      <c r="G73" s="69" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="61"/>
+      <c r="C74" s="62"/>
+      <c r="D74" s="63" t="s">
+        <v>23</v>
+      </c>
+      <c r="E74" s="63" t="s">
+        <v>244</v>
+      </c>
+      <c r="F74" s="70" t="s">
+        <v>247</v>
+      </c>
+      <c r="G74" s="70" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="53" t="s">
+        <v>248</v>
+      </c>
+      <c r="C75" s="54" t="s">
+        <v>209</v>
+      </c>
+      <c r="D75" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="E75" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="F75" s="68" t="s">
+        <v>227</v>
+      </c>
+      <c r="G75" s="68" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="57"/>
+      <c r="C76" s="58"/>
+      <c r="D76" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E76" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="F76" s="69"/>
+      <c r="G76" s="69"/>
+    </row>
+    <row r="77" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="57"/>
+      <c r="C77" s="58"/>
+      <c r="D77" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E77" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="F77" s="69"/>
+      <c r="G77" s="69"/>
+    </row>
+    <row r="78" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="57"/>
+      <c r="C78" s="58"/>
+      <c r="D78" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E78" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="F78" s="69"/>
+      <c r="G78" s="69"/>
+    </row>
+    <row r="79" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="57"/>
+      <c r="C79" s="58"/>
+      <c r="D79" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E79" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F79" s="69"/>
+      <c r="G79" s="69"/>
+    </row>
+    <row r="80" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="57"/>
+      <c r="C80" s="58"/>
+      <c r="D80" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E80" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="F80" s="69"/>
+      <c r="G80" s="69"/>
+    </row>
+    <row r="81" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="57"/>
+      <c r="C81" s="58"/>
+      <c r="D81" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E81" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="F81" s="69"/>
+      <c r="G81" s="69"/>
+    </row>
+    <row r="82" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="57"/>
+      <c r="C82" s="58"/>
+      <c r="D82" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E82" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="F82" s="69"/>
+      <c r="G82" s="69"/>
+    </row>
+    <row r="83" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="57"/>
+      <c r="C83" s="65"/>
+      <c r="D83" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E83" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F83" s="69"/>
+      <c r="G83" s="69"/>
+    </row>
+    <row r="84" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="57"/>
+      <c r="C84" s="66" t="s">
+        <v>214</v>
+      </c>
+      <c r="D84" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E84" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="F84" s="69"/>
+      <c r="G84" s="69"/>
+    </row>
+    <row r="85" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="57"/>
+      <c r="C85" s="58"/>
+      <c r="D85" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E85" s="59" t="s">
+        <v>216</v>
+      </c>
+      <c r="F85" s="69"/>
+      <c r="G85" s="69"/>
+    </row>
+    <row r="86" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="57"/>
+      <c r="C86" s="58"/>
+      <c r="D86" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E86" s="59" t="s">
+        <v>217</v>
+      </c>
+      <c r="F86" s="69"/>
+      <c r="G86" s="69"/>
+    </row>
+    <row r="87" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="57"/>
+      <c r="C87" s="58"/>
+      <c r="D87" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E87" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="F87" s="69"/>
+      <c r="G87" s="69"/>
+    </row>
+    <row r="88" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="57"/>
+      <c r="C88" s="58"/>
+      <c r="D88" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E88" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="F88" s="69"/>
+      <c r="G88" s="69"/>
+    </row>
+    <row r="89" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="57"/>
+      <c r="C89" s="58"/>
+      <c r="D89" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E89" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="F89" s="69"/>
+      <c r="G89" s="69"/>
+    </row>
+    <row r="90" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="57"/>
+      <c r="C90" s="58"/>
+      <c r="D90" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E90" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="F90" s="69"/>
+      <c r="G90" s="69"/>
+    </row>
+    <row r="91" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="57"/>
+      <c r="C91" s="58"/>
+      <c r="D91" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E91" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="F91" s="69"/>
+      <c r="G91" s="69"/>
+    </row>
+    <row r="92" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="57"/>
+      <c r="C92" s="58"/>
+      <c r="D92" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E92" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="F92" s="69"/>
+      <c r="G92" s="69"/>
+    </row>
+    <row r="93" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="57"/>
+      <c r="C93" s="65"/>
+      <c r="D93" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E93" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="F93" s="69"/>
+      <c r="G93" s="69"/>
+    </row>
+    <row r="94" spans="2:7" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B94" s="61"/>
+      <c r="C94" s="67" t="s">
+        <v>250</v>
+      </c>
+      <c r="D94" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="E94" s="63" t="s">
+        <v>249</v>
+      </c>
+      <c r="F94" s="70"/>
+      <c r="G94" s="70"/>
+    </row>
+    <row r="95" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="53" t="s">
+        <v>251</v>
+      </c>
+      <c r="C95" s="54" t="s">
+        <v>209</v>
+      </c>
+      <c r="D95" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="E95" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="F95" s="68" t="s">
+        <v>227</v>
+      </c>
+      <c r="G95" s="68" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="57"/>
+      <c r="C96" s="58"/>
+      <c r="D96" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E96" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="F96" s="69"/>
+      <c r="G96" s="69"/>
+    </row>
+    <row r="97" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="57"/>
+      <c r="C97" s="58"/>
+      <c r="D97" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E97" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="F97" s="69"/>
+      <c r="G97" s="69"/>
+    </row>
+    <row r="98" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="57"/>
+      <c r="C98" s="58"/>
+      <c r="D98" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E98" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="F98" s="69"/>
+      <c r="G98" s="69"/>
+    </row>
+    <row r="99" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="57"/>
+      <c r="C99" s="58"/>
+      <c r="D99" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E99" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F99" s="69"/>
+      <c r="G99" s="69"/>
+    </row>
+    <row r="100" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="57"/>
+      <c r="C100" s="58"/>
+      <c r="D100" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E100" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="F100" s="69"/>
+      <c r="G100" s="69"/>
+    </row>
+    <row r="101" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="57"/>
+      <c r="C101" s="58"/>
+      <c r="D101" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E101" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="F101" s="69"/>
+      <c r="G101" s="69"/>
+    </row>
+    <row r="102" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="57"/>
+      <c r="C102" s="58"/>
+      <c r="D102" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E102" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="F102" s="69"/>
+      <c r="G102" s="69"/>
+    </row>
+    <row r="103" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="57"/>
+      <c r="C103" s="65"/>
+      <c r="D103" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E103" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="F103" s="69"/>
+      <c r="G103" s="69"/>
+    </row>
+    <row r="104" spans="2:7" s="48" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B104" s="57"/>
+      <c r="C104" s="66" t="s">
+        <v>214</v>
+      </c>
+      <c r="D104" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E104" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="F104" s="69"/>
+      <c r="G104" s="69"/>
+    </row>
+    <row r="105" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="57"/>
+      <c r="C105" s="58"/>
+      <c r="D105" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E105" s="59" t="s">
+        <v>216</v>
+      </c>
+      <c r="F105" s="69"/>
+      <c r="G105" s="69"/>
+    </row>
+    <row r="106" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B106" s="57"/>
+      <c r="C106" s="58"/>
+      <c r="D106" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E106" s="59" t="s">
+        <v>217</v>
+      </c>
+      <c r="F106" s="69"/>
+      <c r="G106" s="69"/>
+    </row>
+    <row r="107" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B107" s="57"/>
+      <c r="C107" s="58"/>
+      <c r="D107" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E107" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="F107" s="69"/>
+      <c r="G107" s="69"/>
+    </row>
+    <row r="108" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="57"/>
+      <c r="C108" s="58"/>
+      <c r="D108" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E108" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="F108" s="69"/>
+      <c r="G108" s="69"/>
+    </row>
+    <row r="109" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B109" s="57"/>
+      <c r="C109" s="58"/>
+      <c r="D109" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E109" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="F109" s="69"/>
+      <c r="G109" s="69"/>
+    </row>
+    <row r="110" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B110" s="57"/>
+      <c r="C110" s="58"/>
+      <c r="D110" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E110" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="F110" s="69"/>
+      <c r="G110" s="69"/>
+    </row>
+    <row r="111" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B111" s="57"/>
+      <c r="C111" s="58"/>
+      <c r="D111" s="59" t="s">
+        <v>24</v>
+      </c>
+      <c r="E111" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="F111" s="69"/>
+      <c r="G111" s="69"/>
+    </row>
+    <row r="112" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B112" s="57"/>
+      <c r="C112" s="58"/>
+      <c r="D112" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E112" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="F112" s="69"/>
+      <c r="G112" s="69"/>
+    </row>
+    <row r="113" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B113" s="57"/>
+      <c r="C113" s="65"/>
+      <c r="D113" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E113" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="F113" s="69"/>
+      <c r="G113" s="69"/>
+    </row>
+    <row r="114" spans="2:7" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B114" s="61"/>
+      <c r="C114" s="67" t="s">
+        <v>250</v>
+      </c>
+      <c r="D114" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="E114" s="63" t="s">
+        <v>249</v>
+      </c>
+      <c r="F114" s="70"/>
+      <c r="G114" s="70"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="G36:G56"/>
+    <mergeCell ref="B95:B114"/>
+    <mergeCell ref="C95:C103"/>
+    <mergeCell ref="C104:C113"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F6:F25"/>
+    <mergeCell ref="G6:G25"/>
+    <mergeCell ref="F26:F35"/>
+    <mergeCell ref="G26:G35"/>
+    <mergeCell ref="F36:F56"/>
+    <mergeCell ref="C66:C72"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="B57:B74"/>
+    <mergeCell ref="B75:B94"/>
+    <mergeCell ref="C75:C83"/>
+    <mergeCell ref="C84:C93"/>
+    <mergeCell ref="C57:C65"/>
+    <mergeCell ref="B6:B25"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B26:B35"/>
+    <mergeCell ref="B36:B56"/>
+    <mergeCell ref="C36:C44"/>
+    <mergeCell ref="C45:C51"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="C6:C14"/>
+    <mergeCell ref="C15:C24"/>
+    <mergeCell ref="C26:C35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFE69813-0201-43C0-866C-5D3C128F7149}">
   <dimension ref="A1:BW46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AT1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="AT1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="BA13" sqref="BA13"/>
     </sheetView>
   </sheetViews>

</xml_diff>